<commit_message>
Agregar script y archivo Excel para inventario dinámico
</commit_message>
<xml_diff>
--- a/dynamic_inventory/inventory_data.xlsx
+++ b/dynamic_inventory/inventory_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://colcomerciocom-my.sharepoint.com/personal/1026278709_colcomercio_com_co/Documents/Escritorio/Info Organizada 2024/Proyectos/Ansible/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_AD4D2F04E46CFB4ACB3E20B96556FE32693EDF2F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{244585CC-C43C-4471-80A1-A5783182CC9C}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="11_AD4D2F04E46CFB4ACB3E20B96556FE32693EDF2F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03EBC54D-2DDD-4621-9E67-8C2BDF59A168}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,19 +42,19 @@
     <t>user</t>
   </si>
   <si>
-    <t>10.181.6.38</t>
-  </si>
-  <si>
     <t>lb-security</t>
   </si>
   <si>
-    <t>10.181.6.39</t>
-  </si>
-  <si>
     <t>web-servers</t>
   </si>
   <si>
     <t>ansible</t>
+  </si>
+  <si>
+    <t>10.10.10.1</t>
+  </si>
+  <si>
+    <t>10.10.10.2</t>
   </si>
 </sst>
 </file>
@@ -389,7 +389,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,13 +416,13 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>0</v>
@@ -430,16 +430,16 @@
     </row>
     <row r="3" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>